<commit_message>
Updates to LPF Docs
Updates to LPF Docs
</commit_message>
<xml_diff>
--- a/K9HZ_LPF_Module/K9HZ_LPF_V1.00_BOMs/K9HZ_LPF-Filter_Board_BOM_V1.00_01-10-24.xlsx
+++ b/K9HZ_LPF_Module/K9HZ_LPF_V1.00_BOMs/K9HZ_LPF-Filter_Board_BOM_V1.00_01-10-24.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dad\Documents\GitHub\T41\K9HZ_LPF_Module\K9HZ_LPF_V1.00_BOMs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1D67881-0566-4922-9F20-E6D1BA20263A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E4350F8-8BE5-4DB6-8F2B-CB04D59683B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="190">
   <si>
     <t>Qty</t>
   </si>
@@ -527,40 +527,16 @@
     <t>13 Turns of #20 Wire on a T68-6 Core.</t>
   </si>
   <si>
-    <t>14 Turns of #20 Wire on a T68-6 Core.</t>
-  </si>
-  <si>
     <t>16 Turns of #20 Wire on a T68-6 Core.</t>
   </si>
   <si>
-    <t>17 Turns of #20 Wire on a T68-6 Core.</t>
-  </si>
-  <si>
-    <t>9 Turns of #20 Wire on a T68-17 Core.</t>
-  </si>
-  <si>
-    <t>10 Turns of #20 Wire on a T68-17 Core.</t>
-  </si>
-  <si>
-    <t>29 Turns of #20 Wire on a T68-2 Core.</t>
-  </si>
-  <si>
     <t>30 Turns of #20 Wire on a T68-2 Core.</t>
   </si>
   <si>
-    <t>8 Turns of #20 Wire on a T68-6 Core.</t>
-  </si>
-  <si>
     <t>17 Turns of #20 Wire on a T68-2 Core.</t>
   </si>
   <si>
-    <t>18 Turns of #20 Wire on a T68-2 Core.</t>
-  </si>
-  <si>
     <t>21 Turns of #20 Wire on a T68-2 Core.</t>
-  </si>
-  <si>
-    <t>22 Turns of #20 Wire on a T68-2 Core.</t>
   </si>
   <si>
     <t>T68-2 Cores</t>
@@ -668,7 +644,31 @@
     <t>High</t>
   </si>
   <si>
-    <t>x</t>
+    <t>8 Turns of #20 Wire on a T68-17 Core.</t>
+  </si>
+  <si>
+    <t>7 Turns of #20 Wire on a T68-6 Core.</t>
+  </si>
+  <si>
+    <t>15 Turns of #20 Wire on a T68-6 Core.</t>
+  </si>
+  <si>
+    <t>16 Turns of #20 Wire on a T68-2 Core.</t>
+  </si>
+  <si>
+    <t>20 Turns of #20 Wire on a T68-2 Core.</t>
+  </si>
+  <si>
+    <t>28 Turns of #20 Wire on a T68-2 Core.</t>
+  </si>
+  <si>
+    <t>Final</t>
+  </si>
+  <si>
+    <t>Difference</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        ^ Basis measurements by KI3P</t>
   </si>
 </sst>
 </file>
@@ -843,7 +843,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="42">
+  <fills count="43">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1077,6 +1077,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="12">
     <border>
@@ -1257,7 +1263,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1424,6 +1430,9 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="42" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -1877,7 +1886,7 @@
   <dimension ref="A1:G54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2006,7 +2015,7 @@
         <v>23</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>126</v>
@@ -2292,7 +2301,7 @@
         <v>83</v>
       </c>
       <c r="G29" s="34" t="s">
-        <v>166</v>
+        <v>181</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.35">
@@ -2305,11 +2314,8 @@
       <c r="C30" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="F30" s="34" t="s">
-        <v>126</v>
-      </c>
       <c r="G30" s="34" t="s">
-        <v>167</v>
+        <v>181</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.35">
@@ -2322,11 +2328,8 @@
       <c r="C31" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="F31" s="34" t="s">
-        <v>126</v>
-      </c>
       <c r="G31" s="34" t="s">
-        <v>170</v>
+        <v>182</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.35">
@@ -2339,11 +2342,8 @@
       <c r="C32" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="F32" s="34" t="s">
-        <v>126</v>
-      </c>
       <c r="G32" s="34" t="s">
-        <v>170</v>
+        <v>182</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.35">
@@ -2356,11 +2356,8 @@
       <c r="C33" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="F33" s="34" t="s">
-        <v>126</v>
-      </c>
       <c r="G33" s="34" t="s">
-        <v>170</v>
+        <v>182</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.35">
@@ -2373,11 +2370,8 @@
       <c r="C34" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="F34" s="34" t="s">
-        <v>126</v>
-      </c>
       <c r="G34" s="34" t="s">
-        <v>170</v>
+        <v>182</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.35">
@@ -2390,11 +2384,8 @@
       <c r="C35" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="F35" s="34" t="s">
-        <v>126</v>
-      </c>
       <c r="G35" s="34" t="s">
-        <v>158</v>
+        <v>182</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.35">
@@ -2407,11 +2398,8 @@
       <c r="C36" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="F36" s="34" t="s">
-        <v>126</v>
-      </c>
       <c r="G36" s="34" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.35">
@@ -2424,11 +2412,8 @@
       <c r="C37" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="F37" s="34" t="s">
-        <v>126</v>
-      </c>
       <c r="G37" s="34" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.35">
@@ -2441,11 +2426,8 @@
       <c r="C38" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="F38" s="34" t="s">
-        <v>126</v>
-      </c>
       <c r="G38" s="34" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.35">
@@ -2458,11 +2440,8 @@
       <c r="C39" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="F39" s="34" t="s">
-        <v>126</v>
-      </c>
       <c r="G39" s="34" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.35">
@@ -2475,11 +2454,8 @@
       <c r="C40" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="F40" s="34" t="s">
-        <v>126</v>
-      </c>
       <c r="G40" s="34" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.35">
@@ -2492,11 +2468,8 @@
       <c r="C41" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="F41" s="34" t="s">
-        <v>126</v>
-      </c>
       <c r="G41" s="34" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.35">
@@ -2509,11 +2482,8 @@
       <c r="C42" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="F42" s="34" t="s">
-        <v>126</v>
-      </c>
       <c r="G42" s="34" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.35">
@@ -2526,11 +2496,8 @@
       <c r="C43" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="F43" s="34" t="s">
-        <v>126</v>
-      </c>
       <c r="G43" s="34" t="s">
-        <v>164</v>
+        <v>183</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.35">
@@ -2543,11 +2510,8 @@
       <c r="C44" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="F44" s="34" t="s">
-        <v>126</v>
-      </c>
       <c r="G44" s="34" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.35">
@@ -2560,11 +2524,8 @@
       <c r="C45" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="F45" s="34" t="s">
-        <v>126</v>
-      </c>
       <c r="G45" s="34" t="s">
-        <v>171</v>
+        <v>184</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.35">
@@ -2577,11 +2538,8 @@
       <c r="C46" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="F46" s="34" t="s">
-        <v>126</v>
-      </c>
       <c r="G46" s="34" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.35">
@@ -2594,11 +2552,8 @@
       <c r="C47" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="F47" s="34" t="s">
-        <v>126</v>
-      </c>
       <c r="G47" s="34" t="s">
-        <v>173</v>
+        <v>185</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.35">
@@ -2611,11 +2566,8 @@
       <c r="C48" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="F48" s="34" t="s">
-        <v>126</v>
-      </c>
       <c r="G48" s="34" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.35">
@@ -2628,11 +2580,8 @@
       <c r="C49" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="F49" s="34" t="s">
-        <v>126</v>
-      </c>
       <c r="G49" s="34" t="s">
-        <v>168</v>
+        <v>186</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.35">
@@ -2645,11 +2594,8 @@
       <c r="C50" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="F50" s="34" t="s">
-        <v>126</v>
-      </c>
       <c r="G50" s="34" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.35">
@@ -2658,16 +2604,16 @@
         <v>3</v>
       </c>
       <c r="B51" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="F51" s="34" t="s">
         <v>126</v>
       </c>
       <c r="G51" s="34" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.35">
@@ -2676,13 +2622,13 @@
         <v>21</v>
       </c>
       <c r="B52" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="G52" s="34" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.35">
@@ -2691,13 +2637,13 @@
         <v>9</v>
       </c>
       <c r="B53" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="G53" s="34" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.35">
@@ -2705,13 +2651,13 @@
         <v>38</v>
       </c>
       <c r="B54" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="G54" s="34" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
     </row>
   </sheetData>
@@ -2725,8 +2671,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21315881-8117-4FCF-A08E-B5E61CEF681B}">
   <dimension ref="A1:Z27"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="W26" sqref="W26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="S3" sqref="S3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4871,10 +4817,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DB19532-201D-4964-AA8F-E4D7A92471E4}">
-  <dimension ref="A1:N27"/>
+  <dimension ref="A1:O27"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="Q26" sqref="Q26"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="R5" sqref="R5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4894,7 +4840,7 @@
     <col min="13" max="13" width="6.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>137</v>
       </c>
@@ -4929,13 +4875,19 @@
         <v>156</v>
       </c>
       <c r="L1" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="N1" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="O1" s="4" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" s="4"/>
       <c r="B2" s="4" t="s">
         <v>130</v>
@@ -4961,13 +4913,19 @@
         <v>155</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+        <v>178</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" s="5">
         <v>1</v>
       </c>
@@ -5007,8 +4965,15 @@
       <c r="M3" s="38">
         <v>54</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="N3" s="5">
+        <v>8</v>
+      </c>
+      <c r="O3" s="5">
+        <f>N3-E3</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4" s="16">
         <v>2</v>
       </c>
@@ -5016,7 +4981,7 @@
         <v>0.188</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="D4" s="39" t="s">
         <v>133</v>
@@ -5048,8 +5013,15 @@
       <c r="M4" s="41">
         <v>54</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="N4" s="16">
+        <v>8</v>
+      </c>
+      <c r="O4" s="16">
+        <f t="shared" ref="O4:O24" si="0">N4-E4</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5" s="42">
         <v>1</v>
       </c>
@@ -5089,8 +5061,15 @@
       <c r="M5" s="47">
         <v>30</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="N5" s="5">
+        <v>7</v>
+      </c>
+      <c r="O5" s="5">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A6" s="16">
         <v>2</v>
       </c>
@@ -5130,8 +5109,15 @@
       <c r="M6" s="49">
         <v>30</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="N6" s="16">
+        <v>7</v>
+      </c>
+      <c r="O6" s="16">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A7" s="42">
         <v>2</v>
       </c>
@@ -5171,8 +5157,15 @@
       <c r="M7" s="47">
         <v>24.5</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="N7" s="5">
+        <v>7</v>
+      </c>
+      <c r="O7" s="5">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A8" s="16">
         <v>1</v>
       </c>
@@ -5212,8 +5205,15 @@
       <c r="M8" s="49">
         <v>24.5</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="N8" s="16">
+        <v>7</v>
+      </c>
+      <c r="O8" s="48">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A9" s="42">
         <v>1</v>
       </c>
@@ -5253,8 +5253,15 @@
       <c r="M9" s="47">
         <v>21.5</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="N9" s="5">
+        <v>8</v>
+      </c>
+      <c r="O9" s="5">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A10" s="16">
         <v>2</v>
       </c>
@@ -5262,7 +5269,7 @@
         <v>0.44700000000000001</v>
       </c>
       <c r="C10" s="35" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="D10" s="48" t="s">
         <v>132</v>
@@ -5294,8 +5301,15 @@
       <c r="M10" s="49">
         <v>21.5</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="N10" s="16">
+        <v>9</v>
+      </c>
+      <c r="O10" s="16">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A11" s="42">
         <v>1</v>
       </c>
@@ -5335,8 +5349,15 @@
       <c r="M11" s="47">
         <v>18.5</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="N11" s="5">
+        <v>9</v>
+      </c>
+      <c r="O11" s="5">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A12" s="16">
         <v>2</v>
       </c>
@@ -5344,7 +5365,7 @@
         <v>0.51900000000000002</v>
       </c>
       <c r="C12" s="35" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="D12" s="48" t="s">
         <v>132</v>
@@ -5376,11 +5397,15 @@
       <c r="M12" s="49">
         <v>18.5</v>
       </c>
-      <c r="N12" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="N12" s="16">
+        <v>10</v>
+      </c>
+      <c r="O12" s="16">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A13" s="42">
         <v>1</v>
       </c>
@@ -5420,8 +5445,15 @@
       <c r="M13" s="47">
         <v>14.5</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="N13" s="5">
+        <v>10</v>
+      </c>
+      <c r="O13" s="5">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A14" s="16">
         <v>2</v>
       </c>
@@ -5429,7 +5461,7 @@
         <v>0.67</v>
       </c>
       <c r="C14" s="35" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="D14" s="48" t="s">
         <v>132</v>
@@ -5461,8 +5493,15 @@
       <c r="M14" s="49">
         <v>14.5</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="N14" s="16">
+        <v>11</v>
+      </c>
+      <c r="O14" s="16">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A15" s="42">
         <v>1</v>
       </c>
@@ -5502,8 +5541,15 @@
       <c r="M15" s="47">
         <v>10.3</v>
       </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="N15" s="5">
+        <v>12</v>
+      </c>
+      <c r="O15" s="5">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A16" s="16">
         <v>2</v>
       </c>
@@ -5543,8 +5589,15 @@
       <c r="M16" s="49">
         <v>10.3</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N16" s="16">
+        <v>13</v>
+      </c>
+      <c r="O16" s="16">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A17" s="42">
         <v>1</v>
       </c>
@@ -5584,8 +5637,15 @@
       <c r="M17" s="47">
         <v>7.3</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N17" s="5">
+        <v>15</v>
+      </c>
+      <c r="O17" s="5">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A18" s="16">
         <v>2</v>
       </c>
@@ -5625,8 +5685,15 @@
       <c r="M18" s="49">
         <v>7.3</v>
       </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N18" s="16">
+        <v>16</v>
+      </c>
+      <c r="O18" s="16">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A19" s="42">
         <v>1</v>
       </c>
@@ -5666,8 +5733,15 @@
       <c r="M19" s="52">
         <v>5.5</v>
       </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N19" s="5">
+        <v>16</v>
+      </c>
+      <c r="O19" s="5">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A20" s="16">
         <v>2</v>
       </c>
@@ -5707,8 +5781,15 @@
       <c r="M20" s="53">
         <v>5.5</v>
       </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N20" s="16">
+        <v>17</v>
+      </c>
+      <c r="O20" s="16">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A21" s="42">
         <v>1</v>
       </c>
@@ -5748,8 +5829,15 @@
       <c r="M21" s="52">
         <v>4</v>
       </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N21" s="5">
+        <v>20</v>
+      </c>
+      <c r="O21" s="5">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A22" s="16">
         <v>2</v>
       </c>
@@ -5789,8 +5877,15 @@
       <c r="M22" s="53">
         <v>4</v>
       </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N22" s="16">
+        <v>21</v>
+      </c>
+      <c r="O22" s="16">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A23" s="42">
         <v>1</v>
       </c>
@@ -5830,8 +5925,15 @@
       <c r="M23" s="52">
         <v>2</v>
       </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N23" s="5">
+        <v>28</v>
+      </c>
+      <c r="O23" s="5">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A24" s="16">
         <v>2</v>
       </c>
@@ -5871,11 +5973,18 @@
       <c r="M24" s="53">
         <v>2</v>
       </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N24" s="16">
+        <v>30</v>
+      </c>
+      <c r="O24" s="59">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.35">
       <c r="D25" s="5"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A26" s="4">
         <v>33</v>
       </c>
@@ -5885,8 +5994,11 @@
       <c r="L26" s="5">
         <v>38</v>
       </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N26" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.35">
       <c r="K27" s="5" t="s">
         <v>155</v>
       </c>

</xml_diff>

<commit_message>
Update for V12 Software Release
Update for V12 Software Release
</commit_message>
<xml_diff>
--- a/K9HZ_LPF_Module/K9HZ_LPF_V1.00_BOMs/K9HZ_LPF-Filter_Board_BOM_V1.00_01-10-24.xlsx
+++ b/K9HZ_LPF_Module/K9HZ_LPF_V1.00_BOMs/K9HZ_LPF-Filter_Board_BOM_V1.00_01-10-24.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dad\Documents\GitHub\T41\K9HZ_LPF_Module\K9HZ_LPF_V1.00_BOMs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E4350F8-8BE5-4DB6-8F2B-CB04D59683B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E376634-F0D4-4BB1-8171-9C1A6AB49645}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="T41-WJS-10-band-LPF-filter" sheetId="1" r:id="rId1"/>
@@ -1885,8 +1885,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4819,8 +4819,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DB19532-201D-4964-AA8F-E4D7A92471E4}">
   <dimension ref="A1:O27"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="R5" sqref="R5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S10" sqref="S10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>